<commit_message>
new topic added to contributors.xlsx
</commit_message>
<xml_diff>
--- a/data/contributors.xlsx
+++ b/data/contributors.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="151">
   <si>
     <t>id</t>
   </si>
@@ -332,6 +332,15 @@
     <t>dominant_adpositional_case</t>
   </si>
   <si>
+    <t>Agreement of adpositions with the absolutive/nominative argument</t>
+  </si>
+  <si>
+    <t>June 2022</t>
+  </si>
+  <si>
+    <t>agreement_of_adpositions</t>
+  </si>
+  <si>
     <t>Elevation in the demonstrative system</t>
   </si>
   <si>
@@ -419,12 +428,6 @@
     <t>Ekaterina Matyukhina</t>
   </si>
   <si>
-    <t>Postpositions</t>
-  </si>
-  <si>
-    <t>Tatiana Philippova, Polina Nasledskova</t>
-  </si>
-  <si>
     <t>Predicative possession</t>
   </si>
   <si>
@@ -509,7 +512,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -526,6 +529,9 @@
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -814,7 +820,7 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="3" t="b">
-        <f t="shared" ref="B2:B31" si="1">TRUE()</f>
+        <f t="shared" ref="B2:B32" si="1">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -2115,35 +2121,38 @@
       <c r="A32" s="5">
         <v>31.0</v>
       </c>
-      <c r="B32" s="3"/>
-      <c r="C32" s="1" t="s">
+      <c r="B32" s="3" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="C32" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="D32" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="E32" s="5">
+        <v>2022.0</v>
+      </c>
+      <c r="F32" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="E32" s="1">
-        <v>2020.0</v>
-      </c>
-      <c r="F32" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G32" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H32" s="1" t="s">
+      <c r="G32" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="H32" s="1"/>
+      <c r="I32" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="J32" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="I32" s="1"/>
-      <c r="J32" s="1" t="s">
-        <v>107</v>
-      </c>
       <c r="K32" s="1"/>
-      <c r="L32" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="M32" s="1" t="s">
-        <v>108</v>
+      <c r="L32" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="M32" s="5" t="s">
+        <v>26</v>
       </c>
       <c r="N32" s="1"/>
       <c r="O32" s="1"/>
@@ -2156,10 +2165,10 @@
       </c>
       <c r="B33" s="3"/>
       <c r="C33" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="E33" s="1">
         <v>2020.0</v>
@@ -2171,7 +2180,7 @@
         <v>16</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="I33" s="1"/>
       <c r="J33" s="1" t="s">
@@ -2182,7 +2191,7 @@
         <v>25</v>
       </c>
       <c r="M33" s="1" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="N33" s="1"/>
       <c r="O33" s="1"/>
@@ -2195,10 +2204,10 @@
       </c>
       <c r="B34" s="3"/>
       <c r="C34" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="E34" s="1">
         <v>2020.0</v>
@@ -2210,18 +2219,18 @@
         <v>16</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="I34" s="1"/>
       <c r="J34" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="K34" s="1"/>
       <c r="L34" s="1" t="s">
         <v>25</v>
       </c>
       <c r="M34" s="1" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="N34" s="1"/>
       <c r="O34" s="1"/>
@@ -2232,27 +2241,35 @@
       <c r="A35" s="5">
         <v>34.0</v>
       </c>
-      <c r="B35" s="1"/>
+      <c r="B35" s="3"/>
       <c r="C35" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="E35" s="1">
-        <v>2021.0</v>
-      </c>
-      <c r="F35" s="1"/>
-      <c r="G35" s="1"/>
-      <c r="H35" s="1"/>
+        <v>2020.0</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G35" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>109</v>
+      </c>
       <c r="I35" s="1"/>
-      <c r="J35" s="1"/>
+      <c r="J35" s="1" t="s">
+        <v>115</v>
+      </c>
       <c r="K35" s="1"/>
       <c r="L35" s="1" t="s">
         <v>25</v>
       </c>
       <c r="M35" s="1" t="s">
-        <v>26</v>
+        <v>111</v>
       </c>
       <c r="N35" s="1"/>
       <c r="O35" s="1"/>
@@ -2265,10 +2282,10 @@
       </c>
       <c r="B36" s="1"/>
       <c r="C36" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E36" s="1">
         <v>2021.0</v>
@@ -2280,10 +2297,10 @@
       <c r="J36" s="1"/>
       <c r="K36" s="1"/>
       <c r="L36" s="1" t="s">
-        <v>91</v>
+        <v>25</v>
       </c>
       <c r="M36" s="1" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="N36" s="1"/>
       <c r="O36" s="1"/>
@@ -2296,10 +2313,10 @@
       </c>
       <c r="B37" s="1"/>
       <c r="C37" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E37" s="1">
         <v>2021.0</v>
@@ -2311,10 +2328,10 @@
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
       <c r="L37" s="1" t="s">
-        <v>25</v>
+        <v>91</v>
       </c>
       <c r="M37" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="N37" s="1"/>
       <c r="O37" s="1"/>
@@ -2327,13 +2344,13 @@
       </c>
       <c r="B38" s="1"/>
       <c r="C38" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E38" s="1">
-        <v>2022.0</v>
+        <v>2021.0</v>
       </c>
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
@@ -2342,10 +2359,10 @@
       <c r="J38" s="1"/>
       <c r="K38" s="1"/>
       <c r="L38" s="1" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="M38" s="1" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="N38" s="1"/>
       <c r="O38" s="1"/>
@@ -2358,10 +2375,10 @@
       </c>
       <c r="B39" s="1"/>
       <c r="C39" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E39" s="1">
         <v>2022.0</v>
@@ -2373,7 +2390,7 @@
       <c r="J39" s="1"/>
       <c r="K39" s="1"/>
       <c r="L39" s="1" t="s">
-        <v>91</v>
+        <v>14</v>
       </c>
       <c r="M39" s="1" t="s">
         <v>20</v>
@@ -2389,27 +2406,25 @@
       </c>
       <c r="B40" s="1"/>
       <c r="C40" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="E40" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="F40" s="4" t="s">
-        <v>35</v>
-      </c>
+      <c r="E40" s="1">
+        <v>2022.0</v>
+      </c>
+      <c r="F40" s="1"/>
       <c r="G40" s="1"/>
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
       <c r="J40" s="1"/>
       <c r="K40" s="1"/>
       <c r="L40" s="1" t="s">
-        <v>25</v>
+        <v>91</v>
       </c>
       <c r="M40" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="N40" s="1"/>
       <c r="O40" s="1"/>
@@ -2427,24 +2442,22 @@
       <c r="D41" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="E41" s="1">
-        <v>2022.0</v>
-      </c>
-      <c r="F41" s="1" t="s">
+      <c r="E41" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="G41" s="4" t="s">
-        <v>48</v>
-      </c>
+      <c r="F41" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G41" s="1"/>
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
       <c r="J41" s="1"/>
       <c r="K41" s="1"/>
       <c r="L41" s="1" t="s">
-        <v>129</v>
+        <v>25</v>
       </c>
       <c r="M41" s="1" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="N41" s="1"/>
       <c r="O41" s="1"/>
@@ -2457,23 +2470,29 @@
       </c>
       <c r="B42" s="1"/>
       <c r="C42" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D42" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="D42" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E42" s="1"/>
-      <c r="F42" s="1"/>
-      <c r="G42" s="1"/>
+      <c r="E42" s="1">
+        <v>2022.0</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="G42" s="4" t="s">
+        <v>48</v>
+      </c>
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
       <c r="J42" s="1"/>
       <c r="K42" s="1"/>
       <c r="L42" s="1" t="s">
-        <v>51</v>
+        <v>132</v>
       </c>
       <c r="M42" s="1" t="s">
-        <v>54</v>
+        <v>20</v>
       </c>
       <c r="N42" s="1"/>
       <c r="O42" s="1"/>
@@ -2485,15 +2504,13 @@
         <v>42.0</v>
       </c>
       <c r="B43" s="1"/>
-      <c r="C43" s="5" t="s">
-        <v>131</v>
+      <c r="C43" s="1" t="s">
+        <v>133</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="E43" s="5">
-        <v>2022.0</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="E43" s="1"/>
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
       <c r="H43" s="1"/>
@@ -2501,10 +2518,10 @@
       <c r="J43" s="1"/>
       <c r="K43" s="1"/>
       <c r="L43" s="1" t="s">
-        <v>25</v>
+        <v>51</v>
       </c>
       <c r="M43" s="1" t="s">
-        <v>20</v>
+        <v>54</v>
       </c>
       <c r="N43" s="1"/>
       <c r="O43" s="1"/>
@@ -2516,13 +2533,13 @@
         <v>43.0</v>
       </c>
       <c r="B44" s="1"/>
-      <c r="C44" s="1" t="s">
-        <v>133</v>
+      <c r="C44" s="5" t="s">
+        <v>134</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="E44" s="1">
+        <v>135</v>
+      </c>
+      <c r="E44" s="5">
         <v>2022.0</v>
       </c>
       <c r="F44" s="1"/>
@@ -2530,14 +2547,12 @@
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
       <c r="J44" s="1"/>
-      <c r="K44" s="4" t="s">
-        <v>85</v>
-      </c>
+      <c r="K44" s="1"/>
       <c r="L44" s="1" t="s">
-        <v>101</v>
+        <v>25</v>
       </c>
       <c r="M44" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="N44" s="1"/>
       <c r="O44" s="1"/>
@@ -2550,7 +2565,7 @@
       </c>
       <c r="B45" s="1"/>
       <c r="C45" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>22</v>
@@ -2579,13 +2594,13 @@
       </c>
       <c r="B46" s="1"/>
       <c r="C46" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="E46" s="6" t="s">
-        <v>125</v>
+        <v>138</v>
+      </c>
+      <c r="E46" s="7" t="s">
+        <v>128</v>
       </c>
       <c r="F46" s="1" t="s">
         <v>48</v>
@@ -2612,10 +2627,10 @@
       </c>
       <c r="B47" s="1"/>
       <c r="C47" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E47" s="1">
         <v>2021.0</v>
@@ -2643,10 +2658,10 @@
       </c>
       <c r="B48" s="1"/>
       <c r="C48" s="1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
@@ -2672,10 +2687,10 @@
       </c>
       <c r="B49" s="1"/>
       <c r="C49" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
@@ -2701,10 +2716,10 @@
       </c>
       <c r="B50" s="1"/>
       <c r="C50" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E50" s="1">
         <v>2022.0</v>
@@ -2732,10 +2747,10 @@
       </c>
       <c r="B51" s="1"/>
       <c r="C51" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E51" s="1">
         <v>2022.0</v>
@@ -2763,10 +2778,10 @@
       </c>
       <c r="B52" s="1"/>
       <c r="C52" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E52" s="1"/>
       <c r="F52" s="1"/>
@@ -2776,7 +2791,7 @@
       <c r="J52" s="1"/>
       <c r="K52" s="1"/>
       <c r="L52" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="M52" s="1" t="s">
         <v>20</v>

</xml_diff>

<commit_message>
updated contributors with new finished chapter
</commit_message>
<xml_diff>
--- a/data/contributors.xlsx
+++ b/data/contributors.xlsx
@@ -6,19 +6,19 @@
     <sheet state="visible" name="merged" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">merged!$A$1:$M$52</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">merged!$A$1:$M$53</definedName>
   </definedNames>
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7miA90Tbav2gJ76l4NxDV25zWxA5Zw=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mhSyg0mYMEh74fYbbmfeyjAUAMcaA=="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="154">
   <si>
     <t>id</t>
   </si>
@@ -386,10 +386,19 @@
     <t>Varvara Popova, Rita Popova</t>
   </si>
   <si>
-    <t>Days after today and before yesterday</t>
+    <t>Days after today</t>
   </si>
   <si>
     <t>Timofey Dedov</t>
+  </si>
+  <si>
+    <t>days_after_today</t>
+  </si>
+  <si>
+    <t>Days before today</t>
+  </si>
+  <si>
+    <t>days_before_today</t>
   </si>
   <si>
     <t>Infinitive in the tense-aspect system</t>
@@ -2373,8 +2382,10 @@
       <c r="A39" s="5">
         <v>38.0</v>
       </c>
-      <c r="B39" s="1"/>
-      <c r="C39" s="1" t="s">
+      <c r="B39" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="C39" s="5" t="s">
         <v>122</v>
       </c>
       <c r="D39" s="1" t="s">
@@ -2383,11 +2394,19 @@
       <c r="E39" s="1">
         <v>2022.0</v>
       </c>
-      <c r="F39" s="1"/>
-      <c r="G39" s="1"/>
-      <c r="H39" s="1"/>
+      <c r="F39" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="G39" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="H39" s="5" t="s">
+        <v>36</v>
+      </c>
       <c r="I39" s="1"/>
-      <c r="J39" s="1"/>
+      <c r="J39" s="5" t="s">
+        <v>124</v>
+      </c>
       <c r="K39" s="1"/>
       <c r="L39" s="1" t="s">
         <v>14</v>
@@ -2402,26 +2421,34 @@
     </row>
     <row r="40" ht="12.75" customHeight="1">
       <c r="A40" s="5">
-        <v>39.0</v>
-      </c>
-      <c r="B40" s="1"/>
-      <c r="C40" s="1" t="s">
-        <v>124</v>
+        <v>52.0</v>
+      </c>
+      <c r="B40" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>125</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E40" s="1">
         <v>2022.0</v>
       </c>
-      <c r="F40" s="1"/>
+      <c r="F40" s="5" t="s">
+        <v>100</v>
+      </c>
       <c r="G40" s="1"/>
-      <c r="H40" s="1"/>
+      <c r="H40" s="5" t="s">
+        <v>36</v>
+      </c>
       <c r="I40" s="1"/>
-      <c r="J40" s="1"/>
+      <c r="J40" s="5" t="s">
+        <v>126</v>
+      </c>
       <c r="K40" s="1"/>
       <c r="L40" s="1" t="s">
-        <v>91</v>
+        <v>14</v>
       </c>
       <c r="M40" s="1" t="s">
         <v>20</v>
@@ -2433,31 +2460,29 @@
     </row>
     <row r="41" ht="12.75" customHeight="1">
       <c r="A41" s="5">
-        <v>40.0</v>
+        <v>39.0</v>
       </c>
       <c r="B41" s="1"/>
       <c r="C41" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="E41" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="F41" s="4" t="s">
-        <v>35</v>
-      </c>
+      <c r="E41" s="1">
+        <v>2022.0</v>
+      </c>
+      <c r="F41" s="1"/>
       <c r="G41" s="1"/>
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
       <c r="J41" s="1"/>
       <c r="K41" s="1"/>
       <c r="L41" s="1" t="s">
-        <v>25</v>
+        <v>91</v>
       </c>
       <c r="M41" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="N41" s="1"/>
       <c r="O41" s="1"/>
@@ -2466,7 +2491,7 @@
     </row>
     <row r="42" ht="12.75" customHeight="1">
       <c r="A42" s="5">
-        <v>41.0</v>
+        <v>40.0</v>
       </c>
       <c r="B42" s="1"/>
       <c r="C42" s="1" t="s">
@@ -2475,24 +2500,22 @@
       <c r="D42" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="E42" s="1">
-        <v>2022.0</v>
-      </c>
-      <c r="F42" s="1" t="s">
+      <c r="E42" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="G42" s="4" t="s">
-        <v>48</v>
-      </c>
+      <c r="F42" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G42" s="1"/>
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
       <c r="J42" s="1"/>
       <c r="K42" s="1"/>
       <c r="L42" s="1" t="s">
-        <v>132</v>
+        <v>25</v>
       </c>
       <c r="M42" s="1" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="N42" s="1"/>
       <c r="O42" s="1"/>
@@ -2501,27 +2524,33 @@
     </row>
     <row r="43" ht="12.75" customHeight="1">
       <c r="A43" s="5">
-        <v>42.0</v>
+        <v>41.0</v>
       </c>
       <c r="B43" s="1"/>
       <c r="C43" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D43" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="D43" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E43" s="1"/>
-      <c r="F43" s="1"/>
-      <c r="G43" s="1"/>
+      <c r="E43" s="1">
+        <v>2022.0</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="G43" s="4" t="s">
+        <v>48</v>
+      </c>
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
       <c r="J43" s="1"/>
       <c r="K43" s="1"/>
       <c r="L43" s="1" t="s">
-        <v>51</v>
+        <v>135</v>
       </c>
       <c r="M43" s="1" t="s">
-        <v>54</v>
+        <v>20</v>
       </c>
       <c r="N43" s="1"/>
       <c r="O43" s="1"/>
@@ -2530,18 +2559,16 @@
     </row>
     <row r="44" ht="12.75" customHeight="1">
       <c r="A44" s="5">
-        <v>43.0</v>
+        <v>42.0</v>
       </c>
       <c r="B44" s="1"/>
-      <c r="C44" s="5" t="s">
-        <v>134</v>
+      <c r="C44" s="1" t="s">
+        <v>136</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="E44" s="5">
-        <v>2022.0</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="E44" s="1"/>
       <c r="F44" s="1"/>
       <c r="G44" s="1"/>
       <c r="H44" s="1"/>
@@ -2549,10 +2576,10 @@
       <c r="J44" s="1"/>
       <c r="K44" s="1"/>
       <c r="L44" s="1" t="s">
-        <v>25</v>
+        <v>51</v>
       </c>
       <c r="M44" s="1" t="s">
-        <v>20</v>
+        <v>54</v>
       </c>
       <c r="N44" s="1"/>
       <c r="O44" s="1"/>
@@ -2561,16 +2588,18 @@
     </row>
     <row r="45" ht="12.75" customHeight="1">
       <c r="A45" s="5">
-        <v>44.0</v>
+        <v>43.0</v>
       </c>
       <c r="B45" s="1"/>
-      <c r="C45" s="1" t="s">
-        <v>136</v>
+      <c r="C45" s="5" t="s">
+        <v>137</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E45" s="1"/>
+        <v>138</v>
+      </c>
+      <c r="E45" s="5">
+        <v>2022.0</v>
+      </c>
       <c r="F45" s="1"/>
       <c r="G45" s="1"/>
       <c r="H45" s="1"/>
@@ -2581,7 +2610,7 @@
         <v>25</v>
       </c>
       <c r="M45" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="N45" s="1"/>
       <c r="O45" s="1"/>
@@ -2590,21 +2619,17 @@
     </row>
     <row r="46" ht="12.75" customHeight="1">
       <c r="A46" s="5">
-        <v>45.0</v>
+        <v>44.0</v>
       </c>
       <c r="B46" s="1"/>
       <c r="C46" s="1" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="E46" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="F46" s="1" t="s">
-        <v>48</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="E46" s="1"/>
+      <c r="F46" s="1"/>
       <c r="G46" s="1"/>
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
@@ -2614,7 +2639,7 @@
         <v>25</v>
       </c>
       <c r="M46" s="1" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="N46" s="1"/>
       <c r="O46" s="1"/>
@@ -2623,26 +2648,28 @@
     </row>
     <row r="47" ht="12.75" customHeight="1">
       <c r="A47" s="5">
-        <v>46.0</v>
+        <v>45.0</v>
       </c>
       <c r="B47" s="1"/>
       <c r="C47" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="E47" s="1">
-        <v>2021.0</v>
-      </c>
-      <c r="F47" s="1"/>
+        <v>141</v>
+      </c>
+      <c r="E47" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>48</v>
+      </c>
       <c r="G47" s="1"/>
       <c r="H47" s="1"/>
       <c r="I47" s="1"/>
       <c r="J47" s="1"/>
       <c r="K47" s="1"/>
       <c r="L47" s="1" t="s">
-        <v>91</v>
+        <v>25</v>
       </c>
       <c r="M47" s="1" t="s">
         <v>20</v>
@@ -2654,16 +2681,18 @@
     </row>
     <row r="48" ht="12.75" customHeight="1">
       <c r="A48" s="5">
-        <v>47.0</v>
+        <v>46.0</v>
       </c>
       <c r="B48" s="1"/>
       <c r="C48" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="E48" s="1"/>
+        <v>143</v>
+      </c>
+      <c r="E48" s="1">
+        <v>2021.0</v>
+      </c>
       <c r="F48" s="1"/>
       <c r="G48" s="1"/>
       <c r="H48" s="1"/>
@@ -2671,10 +2700,10 @@
       <c r="J48" s="1"/>
       <c r="K48" s="1"/>
       <c r="L48" s="1" t="s">
-        <v>51</v>
+        <v>91</v>
       </c>
       <c r="M48" s="1" t="s">
-        <v>54</v>
+        <v>20</v>
       </c>
       <c r="N48" s="1"/>
       <c r="O48" s="1"/>
@@ -2683,14 +2712,14 @@
     </row>
     <row r="49" ht="12.75" customHeight="1">
       <c r="A49" s="5">
-        <v>48.0</v>
+        <v>47.0</v>
       </c>
       <c r="B49" s="1"/>
       <c r="C49" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
@@ -2700,10 +2729,10 @@
       <c r="J49" s="1"/>
       <c r="K49" s="1"/>
       <c r="L49" s="1" t="s">
-        <v>25</v>
+        <v>51</v>
       </c>
       <c r="M49" s="1" t="s">
-        <v>26</v>
+        <v>54</v>
       </c>
       <c r="N49" s="1"/>
       <c r="O49" s="1"/>
@@ -2712,18 +2741,16 @@
     </row>
     <row r="50" ht="12.75" customHeight="1">
       <c r="A50" s="5">
-        <v>49.0</v>
+        <v>48.0</v>
       </c>
       <c r="B50" s="1"/>
       <c r="C50" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="E50" s="1">
-        <v>2022.0</v>
-      </c>
+        <v>147</v>
+      </c>
+      <c r="E50" s="1"/>
       <c r="F50" s="1"/>
       <c r="G50" s="1"/>
       <c r="H50" s="1"/>
@@ -2743,14 +2770,14 @@
     </row>
     <row r="51" ht="12.75" customHeight="1">
       <c r="A51" s="5">
-        <v>50.0</v>
+        <v>49.0</v>
       </c>
       <c r="B51" s="1"/>
       <c r="C51" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="E51" s="1">
         <v>2022.0</v>
@@ -2762,7 +2789,7 @@
       <c r="J51" s="1"/>
       <c r="K51" s="1"/>
       <c r="L51" s="1" t="s">
-        <v>91</v>
+        <v>25</v>
       </c>
       <c r="M51" s="1" t="s">
         <v>26</v>
@@ -2774,16 +2801,18 @@
     </row>
     <row r="52" ht="12.75" customHeight="1">
       <c r="A52" s="5">
-        <v>51.0</v>
+        <v>50.0</v>
       </c>
       <c r="B52" s="1"/>
       <c r="C52" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="E52" s="1"/>
+        <v>151</v>
+      </c>
+      <c r="E52" s="1">
+        <v>2022.0</v>
+      </c>
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
       <c r="H52" s="1"/>
@@ -2791,10 +2820,10 @@
       <c r="J52" s="1"/>
       <c r="K52" s="1"/>
       <c r="L52" s="1" t="s">
-        <v>150</v>
+        <v>91</v>
       </c>
       <c r="M52" s="1" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="N52" s="1"/>
       <c r="O52" s="1"/>
@@ -2802,10 +2831,16 @@
       <c r="Q52" s="2"/>
     </row>
     <row r="53" ht="12.75" customHeight="1">
-      <c r="A53" s="2"/>
+      <c r="A53" s="5">
+        <v>51.0</v>
+      </c>
       <c r="B53" s="1"/>
-      <c r="C53" s="1"/>
-      <c r="D53" s="1"/>
+      <c r="C53" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>153</v>
+      </c>
       <c r="E53" s="1"/>
       <c r="F53" s="1"/>
       <c r="G53" s="1"/>
@@ -2813,8 +2848,12 @@
       <c r="I53" s="1"/>
       <c r="J53" s="1"/>
       <c r="K53" s="1"/>
-      <c r="L53" s="1"/>
-      <c r="M53" s="1"/>
+      <c r="L53" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="M53" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="N53" s="1"/>
       <c r="O53" s="1"/>
       <c r="P53" s="2"/>
@@ -6601,7 +6640,7 @@
       <c r="P252" s="2"/>
       <c r="Q252" s="2"/>
     </row>
-    <row r="253" ht="15.75" customHeight="1">
+    <row r="253" ht="12.75" customHeight="1">
       <c r="A253" s="2"/>
       <c r="B253" s="1"/>
       <c r="C253" s="1"/>
@@ -20832,8 +20871,27 @@
       <c r="P1001" s="2"/>
       <c r="Q1001" s="2"/>
     </row>
+    <row r="1002" ht="15.75" customHeight="1">
+      <c r="A1002" s="2"/>
+      <c r="B1002" s="1"/>
+      <c r="C1002" s="1"/>
+      <c r="D1002" s="1"/>
+      <c r="E1002" s="1"/>
+      <c r="F1002" s="1"/>
+      <c r="G1002" s="1"/>
+      <c r="H1002" s="1"/>
+      <c r="I1002" s="1"/>
+      <c r="J1002" s="1"/>
+      <c r="K1002" s="1"/>
+      <c r="L1002" s="1"/>
+      <c r="M1002" s="1"/>
+      <c r="N1002" s="1"/>
+      <c r="O1002" s="1"/>
+      <c r="P1002" s="2"/>
+      <c r="Q1002" s="2"/>
+    </row>
   </sheetData>
-  <autoFilter ref="$A$1:$M$52"/>
+  <autoFilter ref="$A$1:$M$53"/>
   <printOptions/>
   <pageMargins bottom="1.05277777777778" footer="0.0" header="0.0" left="0.7875" right="0.7875" top="1.05277777777778"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
update distributive; update testing
</commit_message>
<xml_diff>
--- a/data/contributors.xlsx
+++ b/data/contributors.xlsx
@@ -448,16 +448,16 @@
     <t xml:space="preserve">numeral_ordinals</t>
   </si>
   <si>
+    <t xml:space="preserve">Derivation of distributives</t>
+  </si>
+  <si>
+    <t xml:space="preserve">numeral_distributives</t>
+  </si>
+  <si>
     <t xml:space="preserve">Root for ‘hundred’</t>
   </si>
   <si>
     <t xml:space="preserve">numeral_root_hundred</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Derivation of distributives</t>
-  </si>
-  <si>
-    <t xml:space="preserve">numeral_distributives</t>
   </si>
   <si>
     <t xml:space="preserve">Numeral systems</t>
@@ -720,7 +720,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
+      <selection pane="bottomLeft" activeCell="B48" activeCellId="0" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -730,7 +730,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="44.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="33.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="11.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="1" width="14.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="1" width="14.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="17.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="11.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="28.76"/>
@@ -3268,7 +3268,10 @@
       <c r="A49" s="2" t="n">
         <v>48</v>
       </c>
-      <c r="B49" s="4"/>
+      <c r="B49" s="4" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
       <c r="C49" s="2" t="s">
         <v>143</v>
       </c>
@@ -30344,7 +30347,7 @@
       <c r="Y1014" s="3"/>
       <c r="Z1014" s="3"/>
     </row>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <autoFilter ref="A1:M67"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
update after Samira's changes
</commit_message>
<xml_diff>
--- a/data/contributors.xlsx
+++ b/data/contributors.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="183">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -720,7 +720,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B48" activeCellId="0" sqref="B48"/>
+      <selection pane="bottomLeft" activeCell="K30" activeCellId="0" sqref="K30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2551,9 +2551,8 @@
       <c r="J35" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="K35" s="2" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+      <c r="K35" s="5" t="s">
+        <v>85</v>
       </c>
       <c r="L35" s="2" t="s">
         <v>116</v>

</xml_diff>

<commit_message>
add numeral base chapter
</commit_message>
<xml_diff>
--- a/data/contributors.xlsx
+++ b/data/contributors.xlsx
@@ -11,7 +11,7 @@
     <sheet name="merged" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">merged!$A$1:$N$76</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">merged!$A$1:$N$77</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="211">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -502,6 +502,18 @@
     <t xml:space="preserve">causatives</t>
   </si>
   <si>
+    <t xml:space="preserve">Numeral Bases</t>
+  </si>
+  <si>
+    <t xml:space="preserve">September 2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">numeral_bases</t>
+  </si>
+  <si>
+    <t xml:space="preserve">?</t>
+  </si>
+  <si>
     <t xml:space="preserve">Causatives: the causee encoding</t>
   </si>
   <si>
@@ -895,12 +907,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AA995"/>
+  <dimension ref="A1:AA996"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E24" activeCellId="0" sqref="E24"/>
+      <selection pane="bottomLeft" activeCell="A52" activeCellId="0" sqref="A52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -910,7 +922,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="44.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="33.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="11.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="14.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="14.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="17.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="11.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="28.76"/>
@@ -3753,29 +3765,46 @@
       <c r="AA51" s="3"/>
     </row>
     <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A52" s="2"/>
-      <c r="B52" s="2"/>
-      <c r="C52" s="10" t="s">
+      <c r="A52" s="2" t="n">
+        <v>51</v>
+      </c>
+      <c r="B52" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="C52" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="D52" s="10" t="s">
+      <c r="D52" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="F52" s="2" t="n">
+        <v>2023</v>
+      </c>
+      <c r="G52" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="E52" s="2"/>
-      <c r="F52" s="2" t="n">
-        <v>2022</v>
-      </c>
-      <c r="G52" s="2"/>
-      <c r="H52" s="2"/>
-      <c r="I52" s="2"/>
-      <c r="J52" s="2"/>
-      <c r="K52" s="2"/>
+      <c r="H52" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="I52" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J52" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="K52" s="2" t="s">
+        <v>161</v>
+      </c>
       <c r="L52" s="2"/>
       <c r="M52" s="2" t="s">
-        <v>27</v>
+        <v>162</v>
       </c>
       <c r="N52" s="2" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="O52" s="2"/>
       <c r="P52" s="2"/>
@@ -3794,15 +3823,15 @@
     <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="2"/>
       <c r="B53" s="2"/>
-      <c r="C53" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="D53" s="2" t="s">
-        <v>24</v>
+      <c r="C53" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="D53" s="10" t="s">
+        <v>164</v>
       </c>
       <c r="E53" s="2"/>
       <c r="F53" s="2" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="G53" s="2"/>
       <c r="H53" s="2"/>
@@ -3814,7 +3843,7 @@
         <v>27</v>
       </c>
       <c r="N53" s="2" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="O53" s="2"/>
       <c r="P53" s="2"/>
@@ -3834,10 +3863,10 @@
       <c r="A54" s="2"/>
       <c r="B54" s="2"/>
       <c r="C54" s="2" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>163</v>
+        <v>24</v>
       </c>
       <c r="E54" s="2"/>
       <c r="F54" s="2" t="n">
@@ -3850,10 +3879,10 @@
       <c r="K54" s="2"/>
       <c r="L54" s="2"/>
       <c r="M54" s="2" t="s">
-        <v>93</v>
+        <v>27</v>
       </c>
       <c r="N54" s="2" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="O54" s="2"/>
       <c r="P54" s="2"/>
@@ -3873,13 +3902,15 @@
       <c r="A55" s="2"/>
       <c r="B55" s="2"/>
       <c r="C55" s="2" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="E55" s="2"/>
-      <c r="F55" s="2"/>
+      <c r="F55" s="2" t="n">
+        <v>2021</v>
+      </c>
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
       <c r="I55" s="2"/>
@@ -3887,10 +3918,10 @@
       <c r="K55" s="2"/>
       <c r="L55" s="2"/>
       <c r="M55" s="2" t="s">
-        <v>27</v>
+        <v>93</v>
       </c>
       <c r="N55" s="2" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="O55" s="2"/>
       <c r="P55" s="2"/>
@@ -3910,15 +3941,13 @@
       <c r="A56" s="2"/>
       <c r="B56" s="2"/>
       <c r="C56" s="2" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="E56" s="2"/>
-      <c r="F56" s="2" t="n">
-        <v>2022</v>
-      </c>
+      <c r="F56" s="2"/>
       <c r="G56" s="2"/>
       <c r="H56" s="2"/>
       <c r="I56" s="2"/>
@@ -3949,10 +3978,10 @@
       <c r="A57" s="2"/>
       <c r="B57" s="2"/>
       <c r="C57" s="2" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="E57" s="2"/>
       <c r="F57" s="2" t="n">
@@ -3965,7 +3994,7 @@
       <c r="K57" s="2"/>
       <c r="L57" s="2"/>
       <c r="M57" s="2" t="s">
-        <v>93</v>
+        <v>27</v>
       </c>
       <c r="N57" s="2" t="s">
         <v>28</v>
@@ -3988,13 +4017,15 @@
       <c r="A58" s="2"/>
       <c r="B58" s="2"/>
       <c r="C58" s="2" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="E58" s="2"/>
-      <c r="F58" s="2"/>
+      <c r="F58" s="2" t="n">
+        <v>2022</v>
+      </c>
       <c r="G58" s="2"/>
       <c r="H58" s="2"/>
       <c r="I58" s="2"/>
@@ -4002,10 +4033,10 @@
       <c r="K58" s="2"/>
       <c r="L58" s="2"/>
       <c r="M58" s="2" t="s">
-        <v>171</v>
+        <v>93</v>
       </c>
       <c r="N58" s="2" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="O58" s="2"/>
       <c r="P58" s="2"/>
@@ -4025,28 +4056,24 @@
       <c r="A59" s="2"/>
       <c r="B59" s="2"/>
       <c r="C59" s="2" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="E59" s="2"/>
-      <c r="F59" s="2" t="n">
-        <v>2021</v>
-      </c>
+      <c r="F59" s="2"/>
       <c r="G59" s="2"/>
       <c r="H59" s="2"/>
-      <c r="I59" s="2" t="s">
-        <v>19</v>
-      </c>
+      <c r="I59" s="2"/>
       <c r="J59" s="2"/>
       <c r="K59" s="2"/>
       <c r="L59" s="2"/>
       <c r="M59" s="2" t="s">
-        <v>27</v>
+        <v>175</v>
       </c>
       <c r="N59" s="2" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="O59" s="2"/>
       <c r="P59" s="2"/>
@@ -4066,10 +4093,10 @@
       <c r="A60" s="2"/>
       <c r="B60" s="2"/>
       <c r="C60" s="2" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="E60" s="2"/>
       <c r="F60" s="2" t="n">
@@ -4077,7 +4104,9 @@
       </c>
       <c r="G60" s="2"/>
       <c r="H60" s="2"/>
-      <c r="I60" s="2"/>
+      <c r="I60" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="J60" s="2"/>
       <c r="K60" s="2"/>
       <c r="L60" s="2"/>
@@ -4105,14 +4134,14 @@
       <c r="A61" s="2"/>
       <c r="B61" s="2"/>
       <c r="C61" s="2" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="E61" s="2"/>
       <c r="F61" s="2" t="n">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="G61" s="2"/>
       <c r="H61" s="2"/>
@@ -4121,10 +4150,10 @@
       <c r="K61" s="2"/>
       <c r="L61" s="2"/>
       <c r="M61" s="2" t="s">
-        <v>93</v>
+        <v>27</v>
       </c>
       <c r="N61" s="2" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="O61" s="2"/>
       <c r="P61" s="2"/>
@@ -4144,28 +4173,26 @@
       <c r="A62" s="2"/>
       <c r="B62" s="2"/>
       <c r="C62" s="2" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="E62" s="8"/>
-      <c r="F62" s="8" t="s">
-        <v>180</v>
-      </c>
-      <c r="G62" s="5" t="s">
-        <v>37</v>
-      </c>
+        <v>181</v>
+      </c>
+      <c r="E62" s="2"/>
+      <c r="F62" s="2" t="n">
+        <v>2022</v>
+      </c>
+      <c r="G62" s="2"/>
       <c r="H62" s="2"/>
       <c r="I62" s="2"/>
       <c r="J62" s="2"/>
       <c r="K62" s="2"/>
       <c r="L62" s="2"/>
       <c r="M62" s="2" t="s">
-        <v>27</v>
+        <v>93</v>
       </c>
       <c r="N62" s="2" t="s">
-        <v>181</v>
+        <v>22</v>
       </c>
       <c r="O62" s="2"/>
       <c r="P62" s="2"/>
@@ -4181,7 +4208,7 @@
       <c r="Z62" s="3"/>
       <c r="AA62" s="3"/>
     </row>
-    <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="2"/>
       <c r="B63" s="2"/>
       <c r="C63" s="2" t="s">
@@ -4190,23 +4217,23 @@
       <c r="D63" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="E63" s="2"/>
-      <c r="F63" s="2" t="n">
-        <v>2022</v>
-      </c>
-      <c r="G63" s="2"/>
+      <c r="E63" s="8"/>
+      <c r="F63" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="G63" s="5" t="s">
+        <v>37</v>
+      </c>
       <c r="H63" s="2"/>
-      <c r="I63" s="2" t="s">
-        <v>38</v>
-      </c>
+      <c r="I63" s="2"/>
       <c r="J63" s="2"/>
       <c r="K63" s="2"/>
       <c r="L63" s="2"/>
       <c r="M63" s="2" t="s">
-        <v>53</v>
+        <v>27</v>
       </c>
       <c r="N63" s="2" t="s">
-        <v>28</v>
+        <v>185</v>
       </c>
       <c r="O63" s="2"/>
       <c r="P63" s="2"/>
@@ -4214,22 +4241,22 @@
       <c r="R63" s="2"/>
       <c r="S63" s="2"/>
       <c r="T63" s="2"/>
-      <c r="U63" s="2"/>
-      <c r="V63" s="2"/>
-      <c r="W63" s="2"/>
-      <c r="X63" s="2"/>
-      <c r="Y63" s="2"/>
-      <c r="Z63" s="2"/>
-      <c r="AA63" s="2"/>
+      <c r="U63" s="3"/>
+      <c r="V63" s="3"/>
+      <c r="W63" s="3"/>
+      <c r="X63" s="3"/>
+      <c r="Y63" s="3"/>
+      <c r="Z63" s="3"/>
+      <c r="AA63" s="3"/>
     </row>
     <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="2"/>
       <c r="B64" s="2"/>
       <c r="C64" s="2" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>147</v>
+        <v>187</v>
       </c>
       <c r="E64" s="2"/>
       <c r="F64" s="2" t="n">
@@ -4237,15 +4264,17 @@
       </c>
       <c r="G64" s="2"/>
       <c r="H64" s="2"/>
-      <c r="I64" s="2"/>
+      <c r="I64" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="J64" s="2"/>
       <c r="K64" s="2"/>
       <c r="L64" s="2"/>
       <c r="M64" s="2" t="s">
-        <v>27</v>
+        <v>53</v>
       </c>
       <c r="N64" s="2" t="s">
-        <v>181</v>
+        <v>28</v>
       </c>
       <c r="O64" s="2"/>
       <c r="P64" s="2"/>
@@ -4265,13 +4294,15 @@
       <c r="A65" s="2"/>
       <c r="B65" s="2"/>
       <c r="C65" s="2" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>93</v>
+        <v>147</v>
       </c>
       <c r="E65" s="2"/>
-      <c r="F65" s="2"/>
+      <c r="F65" s="2" t="n">
+        <v>2022</v>
+      </c>
       <c r="G65" s="2"/>
       <c r="H65" s="2"/>
       <c r="I65" s="2"/>
@@ -4279,9 +4310,11 @@
       <c r="K65" s="2"/>
       <c r="L65" s="2"/>
       <c r="M65" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="N65" s="2"/>
+        <v>27</v>
+      </c>
+      <c r="N65" s="2" t="s">
+        <v>185</v>
+      </c>
       <c r="O65" s="2"/>
       <c r="P65" s="2"/>
       <c r="Q65" s="2"/>
@@ -4300,10 +4333,10 @@
       <c r="A66" s="2"/>
       <c r="B66" s="2"/>
       <c r="C66" s="2" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>187</v>
+        <v>93</v>
       </c>
       <c r="E66" s="2"/>
       <c r="F66" s="2"/>
@@ -4314,7 +4347,7 @@
       <c r="K66" s="2"/>
       <c r="L66" s="2"/>
       <c r="M66" s="2" t="s">
-        <v>187</v>
+        <v>93</v>
       </c>
       <c r="N66" s="2"/>
       <c r="O66" s="2"/>
@@ -4335,15 +4368,13 @@
       <c r="A67" s="2"/>
       <c r="B67" s="2"/>
       <c r="C67" s="2" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="E67" s="2"/>
-      <c r="F67" s="2" t="n">
-        <v>2022</v>
-      </c>
+      <c r="F67" s="2"/>
       <c r="G67" s="2"/>
       <c r="H67" s="2"/>
       <c r="I67" s="2"/>
@@ -4351,11 +4382,9 @@
       <c r="K67" s="2"/>
       <c r="L67" s="2"/>
       <c r="M67" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="N67" s="2" t="s">
-        <v>181</v>
-      </c>
+        <v>191</v>
+      </c>
+      <c r="N67" s="2"/>
       <c r="O67" s="2"/>
       <c r="P67" s="2"/>
       <c r="Q67" s="2"/>
@@ -4374,10 +4403,10 @@
       <c r="A68" s="2"/>
       <c r="B68" s="2"/>
       <c r="C68" s="2" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>45</v>
+        <v>193</v>
       </c>
       <c r="E68" s="2"/>
       <c r="F68" s="2" t="n">
@@ -4390,10 +4419,10 @@
       <c r="K68" s="2"/>
       <c r="L68" s="2"/>
       <c r="M68" s="2" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
       <c r="N68" s="2" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="O68" s="2"/>
       <c r="P68" s="2"/>
@@ -4413,10 +4442,10 @@
       <c r="A69" s="2"/>
       <c r="B69" s="2"/>
       <c r="C69" s="2" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>192</v>
+        <v>45</v>
       </c>
       <c r="E69" s="2"/>
       <c r="F69" s="2" t="n">
@@ -4429,10 +4458,10 @@
       <c r="K69" s="2"/>
       <c r="L69" s="2"/>
       <c r="M69" s="2" t="s">
-        <v>93</v>
+        <v>45</v>
       </c>
       <c r="N69" s="2" t="s">
-        <v>28</v>
+        <v>185</v>
       </c>
       <c r="O69" s="2"/>
       <c r="P69" s="2"/>
@@ -4452,10 +4481,10 @@
       <c r="A70" s="2"/>
       <c r="B70" s="2"/>
       <c r="C70" s="2" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="E70" s="2"/>
       <c r="F70" s="2" t="n">
@@ -4487,18 +4516,18 @@
       <c r="Z70" s="2"/>
       <c r="AA70" s="2"/>
     </row>
-    <row r="71" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="2"/>
       <c r="B71" s="2"/>
       <c r="C71" s="2" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="E71" s="2"/>
       <c r="F71" s="2" t="n">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="G71" s="2"/>
       <c r="H71" s="2"/>
@@ -4518,22 +4547,22 @@
       <c r="R71" s="2"/>
       <c r="S71" s="2"/>
       <c r="T71" s="2"/>
-      <c r="U71" s="3"/>
-      <c r="V71" s="3"/>
-      <c r="W71" s="3"/>
-      <c r="X71" s="3"/>
-      <c r="Y71" s="3"/>
-      <c r="Z71" s="3"/>
-      <c r="AA71" s="3"/>
+      <c r="U71" s="2"/>
+      <c r="V71" s="2"/>
+      <c r="W71" s="2"/>
+      <c r="X71" s="2"/>
+      <c r="Y71" s="2"/>
+      <c r="Z71" s="2"/>
+      <c r="AA71" s="2"/>
     </row>
     <row r="72" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="2"/>
       <c r="B72" s="2"/>
       <c r="C72" s="2" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="E72" s="2"/>
       <c r="F72" s="2" t="n">
@@ -4546,10 +4575,10 @@
       <c r="K72" s="2"/>
       <c r="L72" s="2"/>
       <c r="M72" s="2" t="s">
-        <v>45</v>
+        <v>93</v>
       </c>
       <c r="N72" s="2" t="s">
-        <v>181</v>
+        <v>28</v>
       </c>
       <c r="O72" s="2"/>
       <c r="P72" s="2"/>
@@ -4569,10 +4598,10 @@
       <c r="A73" s="2"/>
       <c r="B73" s="2"/>
       <c r="C73" s="2" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="E73" s="2"/>
       <c r="F73" s="2" t="n">
@@ -4580,16 +4609,16 @@
       </c>
       <c r="G73" s="2"/>
       <c r="H73" s="2"/>
-      <c r="I73" s="2" t="s">
-        <v>38</v>
-      </c>
+      <c r="I73" s="2"/>
       <c r="J73" s="2"/>
       <c r="K73" s="2"/>
       <c r="L73" s="2"/>
       <c r="M73" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="N73" s="2"/>
+        <v>45</v>
+      </c>
+      <c r="N73" s="2" t="s">
+        <v>185</v>
+      </c>
       <c r="O73" s="2"/>
       <c r="P73" s="2"/>
       <c r="Q73" s="2"/>
@@ -4608,10 +4637,10 @@
       <c r="A74" s="2"/>
       <c r="B74" s="2"/>
       <c r="C74" s="2" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="E74" s="2"/>
       <c r="F74" s="2" t="n">
@@ -4626,11 +4655,9 @@
       <c r="K74" s="2"/>
       <c r="L74" s="2"/>
       <c r="M74" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="N74" s="2" t="s">
-        <v>28</v>
-      </c>
+        <v>205</v>
+      </c>
+      <c r="N74" s="2"/>
       <c r="O74" s="2"/>
       <c r="P74" s="2"/>
       <c r="Q74" s="2"/>
@@ -4649,10 +4676,10 @@
       <c r="A75" s="2"/>
       <c r="B75" s="2"/>
       <c r="C75" s="2" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>15</v>
+        <v>207</v>
       </c>
       <c r="E75" s="2"/>
       <c r="F75" s="2" t="n">
@@ -4667,9 +4694,11 @@
       <c r="K75" s="2"/>
       <c r="L75" s="2"/>
       <c r="M75" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="N75" s="2"/>
+        <v>53</v>
+      </c>
+      <c r="N75" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="O75" s="2"/>
       <c r="P75" s="2"/>
       <c r="Q75" s="2"/>
@@ -4687,9 +4716,11 @@
     <row r="76" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="2"/>
       <c r="B76" s="2"/>
-      <c r="C76" s="2"/>
+      <c r="C76" s="2" t="s">
+        <v>208</v>
+      </c>
       <c r="D76" s="2" t="s">
-        <v>205</v>
+        <v>15</v>
       </c>
       <c r="E76" s="2"/>
       <c r="F76" s="2" t="n">
@@ -4697,14 +4728,16 @@
       </c>
       <c r="G76" s="2"/>
       <c r="H76" s="2"/>
-      <c r="I76" s="2"/>
+      <c r="I76" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="J76" s="2"/>
       <c r="K76" s="2"/>
       <c r="L76" s="2"/>
-      <c r="M76" s="2"/>
-      <c r="N76" s="2" t="s">
-        <v>206</v>
-      </c>
+      <c r="M76" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="N76" s="2"/>
       <c r="O76" s="2"/>
       <c r="P76" s="2"/>
       <c r="Q76" s="2"/>
@@ -4723,9 +4756,13 @@
       <c r="A77" s="2"/>
       <c r="B77" s="2"/>
       <c r="C77" s="2"/>
-      <c r="D77" s="2"/>
+      <c r="D77" s="2" t="s">
+        <v>209</v>
+      </c>
       <c r="E77" s="2"/>
-      <c r="F77" s="2"/>
+      <c r="F77" s="2" t="n">
+        <v>2023</v>
+      </c>
       <c r="G77" s="2"/>
       <c r="H77" s="2"/>
       <c r="I77" s="2"/>
@@ -4733,7 +4770,9 @@
       <c r="K77" s="2"/>
       <c r="L77" s="2"/>
       <c r="M77" s="2"/>
-      <c r="N77" s="2"/>
+      <c r="N77" s="2" t="s">
+        <v>210</v>
+      </c>
       <c r="O77" s="2"/>
       <c r="P77" s="2"/>
       <c r="Q77" s="2"/>
@@ -10113,7 +10152,7 @@
       <c r="Z262" s="3"/>
       <c r="AA262" s="3"/>
     </row>
-    <row r="263" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="263" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A263" s="2"/>
       <c r="B263" s="2"/>
       <c r="C263" s="2"/>
@@ -31370,8 +31409,37 @@
       <c r="Z995" s="3"/>
       <c r="AA995" s="3"/>
     </row>
+    <row r="996" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A996" s="2"/>
+      <c r="B996" s="2"/>
+      <c r="C996" s="2"/>
+      <c r="D996" s="2"/>
+      <c r="E996" s="2"/>
+      <c r="F996" s="2"/>
+      <c r="G996" s="2"/>
+      <c r="H996" s="2"/>
+      <c r="I996" s="2"/>
+      <c r="J996" s="2"/>
+      <c r="K996" s="2"/>
+      <c r="L996" s="2"/>
+      <c r="M996" s="2"/>
+      <c r="N996" s="2"/>
+      <c r="O996" s="2"/>
+      <c r="P996" s="2"/>
+      <c r="Q996" s="2"/>
+      <c r="R996" s="2"/>
+      <c r="S996" s="2"/>
+      <c r="T996" s="2"/>
+      <c r="U996" s="3"/>
+      <c r="V996" s="3"/>
+      <c r="W996" s="3"/>
+      <c r="X996" s="3"/>
+      <c r="Y996" s="3"/>
+      <c r="Z996" s="3"/>
+      <c r="AA996" s="3"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:N76"/>
+  <autoFilter ref="A1:N77"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0" footer="0"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
add two chapters by Nina and Rita
</commit_message>
<xml_diff>
--- a/data/contributors.xlsx
+++ b/data/contributors.xlsx
@@ -6,19 +6,19 @@
     <sheet state="visible" name="merged" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">merged!$A$1:$N$79</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">merged!$A$1:$N$86</definedName>
   </definedNames>
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="5ocNw4frvLMqVfDZUdIHpzONt+n8uakI0r51i+/xk0A="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="grgJQwpYSzJVQT/s4BgJII8Ian8svfZCKB7FrnXbEOQ="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="675" uniqueCount="234">
   <si>
     <t>id</t>
   </si>
@@ -542,6 +542,45 @@
     <t>number_of_morphological_slots_in_spatial_forms</t>
   </si>
   <si>
+    <t>Jussive</t>
+  </si>
+  <si>
+    <t>February 2024</t>
+  </si>
+  <si>
+    <t>jussive</t>
+  </si>
+  <si>
+    <t>Gender agreement slot in nominal inflectional paradigms</t>
+  </si>
+  <si>
+    <t>Rita Popova</t>
+  </si>
+  <si>
+    <t>gender_agreement_slot</t>
+  </si>
+  <si>
+    <t>Plural marking on imperatives and prohibitives</t>
+  </si>
+  <si>
+    <t>Vasiliy Zerzele</t>
+  </si>
+  <si>
+    <t>plural_marking_on_imperatives</t>
+  </si>
+  <si>
+    <t>Distinction between transitive and intransitive imperatives</t>
+  </si>
+  <si>
+    <t>Maria Starodubtseva</t>
+  </si>
+  <si>
+    <t>Usage of volitional forms in subordinate clauses</t>
+  </si>
+  <si>
+    <t>Pavel Astafyev</t>
+  </si>
+  <si>
     <t>Causatives: the causee encoding</t>
   </si>
   <si>
@@ -579,12 +618,6 @@
   </si>
   <si>
     <t>Timur Maisak, Samira Verhees</t>
-  </si>
-  <si>
-    <t>Class agreement slot in case paradigms</t>
-  </si>
-  <si>
-    <t>Varvara Popova, Rita Popova</t>
   </si>
   <si>
     <t>Infinitive in the tense-aspect system</t>
@@ -638,12 +671,6 @@
     <t>Anastasia Ivanova</t>
   </si>
   <si>
-    <t>Usage of volitional forms in subordinate clauses</t>
-  </si>
-  <si>
-    <t>Pavel Astafyev</t>
-  </si>
-  <si>
     <t>Lexification patterns of the sense 'to work'</t>
   </si>
   <si>
@@ -662,22 +689,37 @@
     <t>Concept 'maize'</t>
   </si>
   <si>
+    <t>Adaptation of verbal borrowings</t>
+  </si>
+  <si>
     <t>Zaira Khalilova</t>
   </si>
   <si>
     <t>Lena</t>
   </si>
   <si>
-    <t>Distinction between transitive and intransitive imperatives</t>
+    <t>Reflexive pronouns</t>
   </si>
   <si>
-    <t>Maria Starodubtseva</t>
+    <t>Dedicated plural agreement on adjectives</t>
   </si>
   <si>
-    <t>Plural marking of imperatives and prohibitives</t>
+    <t>Syllable structure</t>
   </si>
   <si>
-    <t>Vasiliy Zerzele</t>
+    <t>Alena Muravyeva</t>
+  </si>
+  <si>
+    <t>Localizations in spatial paradigms</t>
+  </si>
+  <si>
+    <t>Vladislava Termus</t>
+  </si>
+  <si>
+    <t>Hortatives</t>
+  </si>
+  <si>
+    <t>Negation</t>
   </si>
 </sst>
 </file>
@@ -705,12 +747,18 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -731,7 +779,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -747,7 +795,10 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="1" fillId="3" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -758,6 +809,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2780,16 +2834,16 @@
       <c r="D33" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="E33" s="1" t="s">
+      <c r="E33" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F33" s="1">
+      <c r="F33" s="5">
         <v>2022.0</v>
       </c>
-      <c r="G33" s="1" t="s">
+      <c r="G33" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="H33" s="1" t="s">
+      <c r="H33" s="5" t="s">
         <v>102</v>
       </c>
       <c r="I33" s="1" t="s">
@@ -2834,16 +2888,16 @@
       <c r="D34" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="E34" s="1" t="s">
+      <c r="E34" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F34" s="1">
+      <c r="F34" s="5">
         <v>2022.0</v>
       </c>
-      <c r="G34" s="1" t="s">
+      <c r="G34" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="H34" s="1" t="s">
+      <c r="H34" s="5" t="s">
         <v>102</v>
       </c>
       <c r="I34" s="1" t="s">
@@ -3665,7 +3719,7 @@
       <c r="A49" s="1">
         <v>48.0</v>
       </c>
-      <c r="B49" s="5" t="b">
+      <c r="B49" s="6" t="b">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -3678,13 +3732,13 @@
       <c r="E49" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="F49" s="6">
+      <c r="F49" s="7">
         <v>2023.0</v>
       </c>
-      <c r="G49" s="7" t="s">
+      <c r="G49" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="H49" s="7" t="s">
+      <c r="H49" s="8" t="s">
         <v>148</v>
       </c>
       <c r="I49" s="1" t="s">
@@ -3719,7 +3773,7 @@
       <c r="A50" s="1">
         <v>49.0</v>
       </c>
-      <c r="B50" s="5" t="b">
+      <c r="B50" s="6" t="b">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -3775,7 +3829,7 @@
       <c r="A51" s="1">
         <v>50.0</v>
       </c>
-      <c r="B51" s="5" t="b">
+      <c r="B51" s="6" t="b">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -3829,7 +3883,7 @@
       <c r="A52" s="1">
         <v>51.0</v>
       </c>
-      <c r="B52" s="5" t="b">
+      <c r="B52" s="6" t="b">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -3935,7 +3989,7 @@
       <c r="AA53" s="1"/>
     </row>
     <row r="54" ht="12.75" customHeight="1">
-      <c r="A54" s="8">
+      <c r="A54" s="9">
         <v>53.0</v>
       </c>
       <c r="B54" s="3" t="b">
@@ -3959,11 +4013,11 @@
       <c r="H54" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="I54" s="8" t="s">
+      <c r="I54" s="9" t="s">
         <v>19</v>
       </c>
       <c r="J54" s="1"/>
-      <c r="K54" s="8" t="s">
+      <c r="K54" s="9" t="s">
         <v>169</v>
       </c>
       <c r="L54" s="1"/>
@@ -3988,7 +4042,7 @@
       <c r="AA54" s="2"/>
     </row>
     <row r="55" ht="12.75" customHeight="1">
-      <c r="A55" s="8">
+      <c r="A55" s="9">
         <v>54.0</v>
       </c>
       <c r="B55" s="3" t="b">
@@ -4003,20 +4057,20 @@
       <c r="E55" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="F55" s="8">
+      <c r="F55" s="9">
         <v>2023.0</v>
       </c>
-      <c r="G55" s="8" t="s">
+      <c r="G55" s="9" t="s">
         <v>172</v>
       </c>
-      <c r="H55" s="8" t="s">
+      <c r="H55" s="9" t="s">
         <v>172</v>
       </c>
       <c r="I55" s="1" t="s">
         <v>19</v>
       </c>
       <c r="J55" s="1"/>
-      <c r="K55" s="8" t="s">
+      <c r="K55" s="9" t="s">
         <v>173</v>
       </c>
       <c r="L55" s="1"/>
@@ -4041,29 +4095,43 @@
       <c r="AA55" s="2"/>
     </row>
     <row r="56" ht="12.75" customHeight="1">
-      <c r="A56" s="1"/>
-      <c r="B56" s="1"/>
-      <c r="C56" s="1" t="s">
+      <c r="A56" s="9">
+        <v>55.0</v>
+      </c>
+      <c r="B56" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C56" s="9" t="s">
         <v>174</v>
       </c>
-      <c r="D56" s="1" t="s">
+      <c r="D56" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="F56" s="9">
+        <v>2023.0</v>
+      </c>
+      <c r="G56" s="9" t="s">
         <v>175</v>
       </c>
-      <c r="E56" s="1"/>
-      <c r="F56" s="1">
-        <v>2022.0</v>
-      </c>
-      <c r="G56" s="1"/>
-      <c r="H56" s="1"/>
-      <c r="I56" s="1"/>
+      <c r="H56" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="I56" s="9" t="s">
+        <v>19</v>
+      </c>
       <c r="J56" s="1"/>
-      <c r="K56" s="1"/>
+      <c r="K56" s="9" t="s">
+        <v>176</v>
+      </c>
       <c r="L56" s="1"/>
-      <c r="M56" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="N56" s="1" t="s">
-        <v>22</v>
+      <c r="M56" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="N56" s="9" t="s">
+        <v>28</v>
       </c>
       <c r="O56" s="1"/>
       <c r="P56" s="1"/>
@@ -4080,23 +4148,37 @@
       <c r="AA56" s="2"/>
     </row>
     <row r="57" ht="12.75" customHeight="1">
-      <c r="A57" s="1"/>
-      <c r="B57" s="1"/>
-      <c r="C57" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E57" s="1"/>
-      <c r="F57" s="1">
-        <v>2021.0</v>
-      </c>
-      <c r="G57" s="1"/>
-      <c r="H57" s="1"/>
-      <c r="I57" s="1"/>
+      <c r="A57" s="9">
+        <v>56.0</v>
+      </c>
+      <c r="B57" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C57" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="D57" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="F57" s="9">
+        <v>2023.0</v>
+      </c>
+      <c r="G57" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="H57" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="I57" s="9" t="s">
+        <v>19</v>
+      </c>
       <c r="J57" s="1"/>
-      <c r="K57" s="1"/>
+      <c r="K57" s="9" t="s">
+        <v>179</v>
+      </c>
       <c r="L57" s="1"/>
       <c r="M57" s="1" t="s">
         <v>27</v>
@@ -4119,29 +4201,41 @@
       <c r="AA57" s="2"/>
     </row>
     <row r="58" ht="12.75" customHeight="1">
-      <c r="A58" s="1"/>
+      <c r="A58" s="9">
+        <v>57.0</v>
+      </c>
       <c r="B58" s="1"/>
-      <c r="C58" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="E58" s="1"/>
+      <c r="C58" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="D58" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>116</v>
+      </c>
       <c r="F58" s="1">
-        <v>2021.0</v>
-      </c>
-      <c r="G58" s="1"/>
-      <c r="H58" s="1"/>
-      <c r="I58" s="1"/>
+        <v>2023.0</v>
+      </c>
+      <c r="G58" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="H58" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="I58" s="9" t="s">
+        <v>19</v>
+      </c>
       <c r="J58" s="1"/>
-      <c r="K58" s="1"/>
+      <c r="K58" s="9" t="s">
+        <v>182</v>
+      </c>
       <c r="L58" s="1"/>
       <c r="M58" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="N58" s="1" t="s">
-        <v>22</v>
+        <v>45</v>
+      </c>
+      <c r="N58" s="9" t="s">
+        <v>28</v>
       </c>
       <c r="O58" s="1"/>
       <c r="P58" s="1"/>
@@ -4160,14 +4254,16 @@
     <row r="59" ht="12.75" customHeight="1">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
-      <c r="C59" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>180</v>
+      <c r="C59" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="D59" s="9" t="s">
+        <v>184</v>
       </c>
       <c r="E59" s="1"/>
-      <c r="F59" s="1"/>
+      <c r="F59" s="1">
+        <v>2023.0</v>
+      </c>
       <c r="G59" s="1"/>
       <c r="H59" s="1"/>
       <c r="I59" s="1"/>
@@ -4175,9 +4271,9 @@
       <c r="K59" s="1"/>
       <c r="L59" s="1"/>
       <c r="M59" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="N59" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="N59" s="9" t="s">
         <v>28</v>
       </c>
       <c r="O59" s="1"/>
@@ -4198,14 +4294,14 @@
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="E60" s="1"/>
       <c r="F60" s="1">
-        <v>2022.0</v>
+        <v>2023.0</v>
       </c>
       <c r="G60" s="1"/>
       <c r="H60" s="1"/>
@@ -4214,10 +4310,10 @@
       <c r="K60" s="1"/>
       <c r="L60" s="1"/>
       <c r="M60" s="1" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
       <c r="N60" s="1" t="s">
-        <v>28</v>
+        <v>166</v>
       </c>
       <c r="O60" s="1"/>
       <c r="P60" s="1"/>
@@ -4237,10 +4333,10 @@
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="E61" s="1"/>
       <c r="F61" s="1">
@@ -4253,10 +4349,10 @@
       <c r="K61" s="1"/>
       <c r="L61" s="1"/>
       <c r="M61" s="1" t="s">
-        <v>93</v>
+        <v>27</v>
       </c>
       <c r="N61" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="O61" s="1"/>
       <c r="P61" s="1"/>
@@ -4276,13 +4372,15 @@
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>186</v>
+        <v>24</v>
       </c>
       <c r="E62" s="1"/>
-      <c r="F62" s="1"/>
+      <c r="F62" s="1">
+        <v>2021.0</v>
+      </c>
       <c r="G62" s="1"/>
       <c r="H62" s="1"/>
       <c r="I62" s="1"/>
@@ -4290,10 +4388,10 @@
       <c r="K62" s="1"/>
       <c r="L62" s="1"/>
       <c r="M62" s="1" t="s">
-        <v>186</v>
+        <v>27</v>
       </c>
       <c r="N62" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="O62" s="1"/>
       <c r="P62" s="1"/>
@@ -4313,10 +4411,10 @@
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="E63" s="1"/>
       <c r="F63" s="1">
@@ -4329,10 +4427,10 @@
       <c r="K63" s="1"/>
       <c r="L63" s="1"/>
       <c r="M63" s="1" t="s">
-        <v>27</v>
+        <v>93</v>
       </c>
       <c r="N63" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="O63" s="1"/>
       <c r="P63" s="1"/>
@@ -4352,15 +4450,13 @@
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="E64" s="1"/>
-      <c r="F64" s="1">
-        <v>2022.0</v>
-      </c>
+      <c r="F64" s="1"/>
       <c r="G64" s="1"/>
       <c r="H64" s="1"/>
       <c r="I64" s="1"/>
@@ -4368,10 +4464,10 @@
       <c r="K64" s="1"/>
       <c r="L64" s="1"/>
       <c r="M64" s="1" t="s">
-        <v>93</v>
+        <v>27</v>
       </c>
       <c r="N64" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="O64" s="1"/>
       <c r="P64" s="1"/>
@@ -4391,18 +4487,16 @@
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="E65" s="6"/>
-      <c r="F65" s="6" t="s">
-        <v>193</v>
-      </c>
-      <c r="G65" s="4" t="s">
-        <v>37</v>
-      </c>
+        <v>195</v>
+      </c>
+      <c r="E65" s="1"/>
+      <c r="F65" s="1">
+        <v>2022.0</v>
+      </c>
+      <c r="G65" s="1"/>
       <c r="H65" s="1"/>
       <c r="I65" s="1"/>
       <c r="J65" s="1"/>
@@ -4412,7 +4506,7 @@
         <v>27</v>
       </c>
       <c r="N65" s="1" t="s">
-        <v>166</v>
+        <v>28</v>
       </c>
       <c r="O65" s="1"/>
       <c r="P65" s="1"/>
@@ -4428,14 +4522,14 @@
       <c r="Z65" s="2"/>
       <c r="AA65" s="2"/>
     </row>
-    <row r="66" ht="15.75" customHeight="1">
+    <row r="66" ht="12.75" customHeight="1">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="E66" s="1"/>
       <c r="F66" s="1">
@@ -4443,14 +4537,12 @@
       </c>
       <c r="G66" s="1"/>
       <c r="H66" s="1"/>
-      <c r="I66" s="1" t="s">
-        <v>38</v>
-      </c>
+      <c r="I66" s="1"/>
       <c r="J66" s="1"/>
       <c r="K66" s="1"/>
       <c r="L66" s="1"/>
       <c r="M66" s="1" t="s">
-        <v>53</v>
+        <v>93</v>
       </c>
       <c r="N66" s="1" t="s">
         <v>28</v>
@@ -4461,27 +4553,25 @@
       <c r="R66" s="1"/>
       <c r="S66" s="1"/>
       <c r="T66" s="1"/>
-      <c r="U66" s="1"/>
-      <c r="V66" s="1"/>
-      <c r="W66" s="1"/>
-      <c r="X66" s="1"/>
-      <c r="Y66" s="1"/>
-      <c r="Z66" s="1"/>
-      <c r="AA66" s="1"/>
-    </row>
-    <row r="67" ht="15.75" customHeight="1">
+      <c r="U66" s="2"/>
+      <c r="V66" s="2"/>
+      <c r="W66" s="2"/>
+      <c r="X66" s="2"/>
+      <c r="Y66" s="2"/>
+      <c r="Z66" s="2"/>
+      <c r="AA66" s="2"/>
+    </row>
+    <row r="67" ht="12.75" customHeight="1">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>147</v>
+        <v>199</v>
       </c>
       <c r="E67" s="1"/>
-      <c r="F67" s="1">
-        <v>2022.0</v>
-      </c>
+      <c r="F67" s="1"/>
       <c r="G67" s="1"/>
       <c r="H67" s="1"/>
       <c r="I67" s="1"/>
@@ -4489,10 +4579,10 @@
       <c r="K67" s="1"/>
       <c r="L67" s="1"/>
       <c r="M67" s="1" t="s">
-        <v>27</v>
+        <v>199</v>
       </c>
       <c r="N67" s="1" t="s">
-        <v>166</v>
+        <v>22</v>
       </c>
       <c r="O67" s="1"/>
       <c r="P67" s="1"/>
@@ -4500,25 +4590,27 @@
       <c r="R67" s="1"/>
       <c r="S67" s="1"/>
       <c r="T67" s="1"/>
-      <c r="U67" s="1"/>
-      <c r="V67" s="1"/>
-      <c r="W67" s="1"/>
-      <c r="X67" s="1"/>
-      <c r="Y67" s="1"/>
-      <c r="Z67" s="1"/>
-      <c r="AA67" s="1"/>
-    </row>
-    <row r="68" ht="15.75" customHeight="1">
+      <c r="U67" s="2"/>
+      <c r="V67" s="2"/>
+      <c r="W67" s="2"/>
+      <c r="X67" s="2"/>
+      <c r="Y67" s="2"/>
+      <c r="Z67" s="2"/>
+      <c r="AA67" s="2"/>
+    </row>
+    <row r="68" ht="12.75" customHeight="1">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>93</v>
+        <v>201</v>
       </c>
       <c r="E68" s="1"/>
-      <c r="F68" s="1"/>
+      <c r="F68" s="1">
+        <v>2022.0</v>
+      </c>
       <c r="G68" s="1"/>
       <c r="H68" s="1"/>
       <c r="I68" s="1"/>
@@ -4528,64 +4620,72 @@
       <c r="M68" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="N68" s="1"/>
+      <c r="N68" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="O68" s="1"/>
       <c r="P68" s="1"/>
       <c r="Q68" s="1"/>
       <c r="R68" s="1"/>
       <c r="S68" s="1"/>
       <c r="T68" s="1"/>
-      <c r="U68" s="1"/>
-      <c r="V68" s="1"/>
-      <c r="W68" s="1"/>
-      <c r="X68" s="1"/>
-      <c r="Y68" s="1"/>
-      <c r="Z68" s="1"/>
-      <c r="AA68" s="1"/>
-    </row>
-    <row r="69" ht="15.75" customHeight="1">
+      <c r="U68" s="2"/>
+      <c r="V68" s="2"/>
+      <c r="W68" s="2"/>
+      <c r="X68" s="2"/>
+      <c r="Y68" s="2"/>
+      <c r="Z68" s="2"/>
+      <c r="AA68" s="2"/>
+    </row>
+    <row r="69" ht="12.75" customHeight="1">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="E69" s="1"/>
-      <c r="F69" s="1"/>
-      <c r="G69" s="1"/>
+        <v>203</v>
+      </c>
+      <c r="E69" s="7"/>
+      <c r="F69" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="G69" s="4" t="s">
+        <v>37</v>
+      </c>
       <c r="H69" s="1"/>
       <c r="I69" s="1"/>
       <c r="J69" s="1"/>
       <c r="K69" s="1"/>
       <c r="L69" s="1"/>
       <c r="M69" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="N69" s="1"/>
+        <v>27</v>
+      </c>
+      <c r="N69" s="1" t="s">
+        <v>166</v>
+      </c>
       <c r="O69" s="1"/>
       <c r="P69" s="1"/>
       <c r="Q69" s="1"/>
       <c r="R69" s="1"/>
       <c r="S69" s="1"/>
       <c r="T69" s="1"/>
-      <c r="U69" s="1"/>
-      <c r="V69" s="1"/>
-      <c r="W69" s="1"/>
-      <c r="X69" s="1"/>
-      <c r="Y69" s="1"/>
-      <c r="Z69" s="1"/>
-      <c r="AA69" s="1"/>
+      <c r="U69" s="2"/>
+      <c r="V69" s="2"/>
+      <c r="W69" s="2"/>
+      <c r="X69" s="2"/>
+      <c r="Y69" s="2"/>
+      <c r="Z69" s="2"/>
+      <c r="AA69" s="2"/>
     </row>
     <row r="70" ht="15.75" customHeight="1">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>201</v>
+        <v>206</v>
       </c>
       <c r="E70" s="1"/>
       <c r="F70" s="1">
@@ -4593,15 +4693,17 @@
       </c>
       <c r="G70" s="1"/>
       <c r="H70" s="1"/>
-      <c r="I70" s="1"/>
+      <c r="I70" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="J70" s="1"/>
       <c r="K70" s="1"/>
       <c r="L70" s="1"/>
       <c r="M70" s="1" t="s">
-        <v>27</v>
+        <v>53</v>
       </c>
       <c r="N70" s="1" t="s">
-        <v>166</v>
+        <v>28</v>
       </c>
       <c r="O70" s="1"/>
       <c r="P70" s="1"/>
@@ -4621,10 +4723,10 @@
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>203</v>
+        <v>147</v>
       </c>
       <c r="E71" s="1"/>
       <c r="F71" s="1">
@@ -4637,10 +4739,10 @@
       <c r="K71" s="1"/>
       <c r="L71" s="1"/>
       <c r="M71" s="1" t="s">
-        <v>93</v>
+        <v>27</v>
       </c>
       <c r="N71" s="1" t="s">
-        <v>28</v>
+        <v>166</v>
       </c>
       <c r="O71" s="1"/>
       <c r="P71" s="1"/>
@@ -4660,15 +4762,13 @@
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>205</v>
+        <v>93</v>
       </c>
       <c r="E72" s="1"/>
-      <c r="F72" s="1">
-        <v>2022.0</v>
-      </c>
+      <c r="F72" s="1"/>
       <c r="G72" s="1"/>
       <c r="H72" s="1"/>
       <c r="I72" s="1"/>
@@ -4678,9 +4778,7 @@
       <c r="M72" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="N72" s="1" t="s">
-        <v>28</v>
-      </c>
+      <c r="N72" s="1"/>
       <c r="O72" s="1"/>
       <c r="P72" s="1"/>
       <c r="Q72" s="1"/>
@@ -4695,19 +4793,17 @@
       <c r="Z72" s="1"/>
       <c r="AA72" s="1"/>
     </row>
-    <row r="73" ht="12.75" customHeight="1">
+    <row r="73" ht="15.75" customHeight="1">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="E73" s="1"/>
-      <c r="F73" s="1">
-        <v>2023.0</v>
-      </c>
+      <c r="F73" s="1"/>
       <c r="G73" s="1"/>
       <c r="H73" s="1"/>
       <c r="I73" s="1"/>
@@ -4715,87 +4811,83 @@
       <c r="K73" s="1"/>
       <c r="L73" s="1"/>
       <c r="M73" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="N73" s="1" t="s">
-        <v>166</v>
-      </c>
+        <v>210</v>
+      </c>
+      <c r="N73" s="1"/>
       <c r="O73" s="1"/>
       <c r="P73" s="1"/>
       <c r="Q73" s="1"/>
       <c r="R73" s="1"/>
       <c r="S73" s="1"/>
       <c r="T73" s="1"/>
-      <c r="U73" s="2"/>
-      <c r="V73" s="2"/>
-      <c r="W73" s="2"/>
-      <c r="X73" s="2"/>
-      <c r="Y73" s="2"/>
-      <c r="Z73" s="2"/>
-      <c r="AA73" s="2"/>
-    </row>
-    <row r="74" ht="12.75" customHeight="1">
+      <c r="U73" s="1"/>
+      <c r="V73" s="1"/>
+      <c r="W73" s="1"/>
+      <c r="X73" s="1"/>
+      <c r="Y73" s="1"/>
+      <c r="Z73" s="1"/>
+      <c r="AA73" s="1"/>
+    </row>
+    <row r="74" ht="15.75" customHeight="1">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="E74" s="1"/>
       <c r="F74" s="1">
-        <v>2023.0</v>
+        <v>2022.0</v>
       </c>
       <c r="G74" s="1"/>
       <c r="H74" s="1"/>
-      <c r="I74" s="1" t="s">
-        <v>38</v>
-      </c>
+      <c r="I74" s="1"/>
       <c r="J74" s="1"/>
       <c r="K74" s="1"/>
       <c r="L74" s="1"/>
       <c r="M74" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="N74" s="1"/>
+        <v>27</v>
+      </c>
+      <c r="N74" s="1" t="s">
+        <v>166</v>
+      </c>
       <c r="O74" s="1"/>
       <c r="P74" s="1"/>
       <c r="Q74" s="1"/>
       <c r="R74" s="1"/>
       <c r="S74" s="1"/>
       <c r="T74" s="1"/>
-      <c r="U74" s="2"/>
-      <c r="V74" s="2"/>
-      <c r="W74" s="2"/>
-      <c r="X74" s="2"/>
-      <c r="Y74" s="2"/>
-      <c r="Z74" s="2"/>
-      <c r="AA74" s="2"/>
-    </row>
-    <row r="75" ht="12.75" customHeight="1">
+      <c r="U74" s="1"/>
+      <c r="V74" s="1"/>
+      <c r="W74" s="1"/>
+      <c r="X74" s="1"/>
+      <c r="Y74" s="1"/>
+      <c r="Z74" s="1"/>
+      <c r="AA74" s="1"/>
+    </row>
+    <row r="75" ht="15.75" customHeight="1">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="E75" s="1"/>
       <c r="F75" s="1">
-        <v>2023.0</v>
+        <v>2022.0</v>
       </c>
       <c r="G75" s="1"/>
       <c r="H75" s="1"/>
-      <c r="I75" s="1" t="s">
-        <v>38</v>
-      </c>
+      <c r="I75" s="1"/>
       <c r="J75" s="1"/>
       <c r="K75" s="1"/>
       <c r="L75" s="1"/>
       <c r="M75" s="1" t="s">
-        <v>53</v>
+        <v>93</v>
       </c>
       <c r="N75" s="1" t="s">
         <v>28</v>
@@ -4806,59 +4898,61 @@
       <c r="R75" s="1"/>
       <c r="S75" s="1"/>
       <c r="T75" s="1"/>
-      <c r="U75" s="2"/>
-      <c r="V75" s="2"/>
-      <c r="W75" s="2"/>
-      <c r="X75" s="2"/>
-      <c r="Y75" s="2"/>
-      <c r="Z75" s="2"/>
-      <c r="AA75" s="2"/>
-    </row>
-    <row r="76" ht="12.75" customHeight="1">
+      <c r="U75" s="1"/>
+      <c r="V75" s="1"/>
+      <c r="W75" s="1"/>
+      <c r="X75" s="1"/>
+      <c r="Y75" s="1"/>
+      <c r="Z75" s="1"/>
+      <c r="AA75" s="1"/>
+    </row>
+    <row r="76" ht="15.75" customHeight="1">
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>15</v>
+        <v>216</v>
       </c>
       <c r="E76" s="1"/>
       <c r="F76" s="1">
-        <v>2023.0</v>
+        <v>2022.0</v>
       </c>
       <c r="G76" s="1"/>
       <c r="H76" s="1"/>
-      <c r="I76" s="1" t="s">
-        <v>38</v>
-      </c>
+      <c r="I76" s="1"/>
       <c r="J76" s="1"/>
       <c r="K76" s="1"/>
       <c r="L76" s="1"/>
       <c r="M76" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="N76" s="1"/>
+        <v>93</v>
+      </c>
+      <c r="N76" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="O76" s="1"/>
       <c r="P76" s="1"/>
       <c r="Q76" s="1"/>
       <c r="R76" s="1"/>
       <c r="S76" s="1"/>
       <c r="T76" s="1"/>
-      <c r="U76" s="2"/>
-      <c r="V76" s="2"/>
-      <c r="W76" s="2"/>
-      <c r="X76" s="2"/>
-      <c r="Y76" s="2"/>
-      <c r="Z76" s="2"/>
-      <c r="AA76" s="2"/>
+      <c r="U76" s="1"/>
+      <c r="V76" s="1"/>
+      <c r="W76" s="1"/>
+      <c r="X76" s="1"/>
+      <c r="Y76" s="1"/>
+      <c r="Z76" s="1"/>
+      <c r="AA76" s="1"/>
     </row>
     <row r="77" ht="12.75" customHeight="1">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
-      <c r="C77" s="1"/>
+      <c r="C77" s="1" t="s">
+        <v>217</v>
+      </c>
       <c r="D77" s="1" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="E77" s="1"/>
       <c r="F77" s="1">
@@ -4866,14 +4960,16 @@
       </c>
       <c r="G77" s="1"/>
       <c r="H77" s="1"/>
-      <c r="I77" s="1"/>
+      <c r="I77" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="J77" s="1"/>
       <c r="K77" s="1"/>
       <c r="L77" s="1"/>
-      <c r="M77" s="1"/>
-      <c r="N77" s="1" t="s">
-        <v>215</v>
-      </c>
+      <c r="M77" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="N77" s="1"/>
       <c r="O77" s="1"/>
       <c r="P77" s="1"/>
       <c r="Q77" s="1"/>
@@ -4891,11 +4987,11 @@
     <row r="78" ht="12.75" customHeight="1">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
-      <c r="C78" s="8" t="s">
-        <v>216</v>
-      </c>
-      <c r="D78" s="8" t="s">
-        <v>217</v>
+      <c r="C78" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>221</v>
       </c>
       <c r="E78" s="1"/>
       <c r="F78" s="1">
@@ -4903,14 +4999,18 @@
       </c>
       <c r="G78" s="1"/>
       <c r="H78" s="1"/>
-      <c r="I78" s="1"/>
+      <c r="I78" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="J78" s="1"/>
       <c r="K78" s="1"/>
       <c r="L78" s="1"/>
       <c r="M78" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="N78" s="1"/>
+        <v>53</v>
+      </c>
+      <c r="N78" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="O78" s="1"/>
       <c r="P78" s="1"/>
       <c r="Q78" s="1"/>
@@ -4928,11 +5028,11 @@
     <row r="79" ht="12.75" customHeight="1">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
-      <c r="C79" s="8" t="s">
-        <v>218</v>
-      </c>
-      <c r="D79" s="8" t="s">
-        <v>219</v>
+      <c r="C79" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="E79" s="1"/>
       <c r="F79" s="1">
@@ -4940,12 +5040,14 @@
       </c>
       <c r="G79" s="1"/>
       <c r="H79" s="1"/>
-      <c r="I79" s="1"/>
+      <c r="I79" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="J79" s="1"/>
       <c r="K79" s="1"/>
       <c r="L79" s="1"/>
       <c r="M79" s="1" t="s">
-        <v>45</v>
+        <v>15</v>
       </c>
       <c r="N79" s="1"/>
       <c r="O79" s="1"/>
@@ -4965,18 +5067,28 @@
     <row r="80" ht="12.75" customHeight="1">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
-      <c r="C80" s="1"/>
-      <c r="D80" s="1"/>
+      <c r="C80" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>224</v>
+      </c>
       <c r="E80" s="1"/>
-      <c r="F80" s="1"/>
+      <c r="F80" s="1">
+        <v>2023.0</v>
+      </c>
       <c r="G80" s="1"/>
       <c r="H80" s="1"/>
       <c r="I80" s="1"/>
       <c r="J80" s="1"/>
       <c r="K80" s="1"/>
       <c r="L80" s="1"/>
-      <c r="M80" s="1"/>
-      <c r="N80" s="1"/>
+      <c r="M80" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="N80" s="1" t="s">
+        <v>225</v>
+      </c>
       <c r="O80" s="1"/>
       <c r="P80" s="1"/>
       <c r="Q80" s="1"/>
@@ -4994,8 +5106,12 @@
     <row r="81" ht="12.75" customHeight="1">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
-      <c r="C81" s="1"/>
-      <c r="D81" s="1"/>
+      <c r="C81" s="9" t="s">
+        <v>226</v>
+      </c>
+      <c r="D81" s="9" t="s">
+        <v>168</v>
+      </c>
       <c r="E81" s="1"/>
       <c r="F81" s="1"/>
       <c r="G81" s="1"/>
@@ -5004,8 +5120,12 @@
       <c r="J81" s="1"/>
       <c r="K81" s="1"/>
       <c r="L81" s="1"/>
-      <c r="M81" s="1"/>
-      <c r="N81" s="1"/>
+      <c r="M81" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="N81" s="9" t="s">
+        <v>28</v>
+      </c>
       <c r="O81" s="1"/>
       <c r="P81" s="1"/>
       <c r="Q81" s="1"/>
@@ -5023,8 +5143,12 @@
     <row r="82" ht="12.75" customHeight="1">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
-      <c r="C82" s="1"/>
-      <c r="D82" s="1"/>
+      <c r="C82" s="9" t="s">
+        <v>227</v>
+      </c>
+      <c r="D82" s="9" t="s">
+        <v>119</v>
+      </c>
       <c r="E82" s="1"/>
       <c r="F82" s="1"/>
       <c r="G82" s="1"/>
@@ -5033,7 +5157,9 @@
       <c r="J82" s="1"/>
       <c r="K82" s="1"/>
       <c r="L82" s="1"/>
-      <c r="M82" s="1"/>
+      <c r="M82" s="9" t="s">
+        <v>119</v>
+      </c>
       <c r="N82" s="1"/>
       <c r="O82" s="1"/>
       <c r="P82" s="1"/>
@@ -5052,17 +5178,25 @@
     <row r="83" ht="12.75" customHeight="1">
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
-      <c r="C83" s="1"/>
-      <c r="D83" s="1"/>
+      <c r="C83" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="D83" s="9" t="s">
+        <v>229</v>
+      </c>
       <c r="E83" s="1"/>
       <c r="F83" s="1"/>
       <c r="G83" s="1"/>
       <c r="H83" s="1"/>
-      <c r="I83" s="1"/>
+      <c r="I83" s="9" t="s">
+        <v>54</v>
+      </c>
       <c r="J83" s="1"/>
       <c r="K83" s="1"/>
       <c r="L83" s="1"/>
-      <c r="M83" s="1"/>
+      <c r="M83" s="9" t="s">
+        <v>53</v>
+      </c>
       <c r="N83" s="1"/>
       <c r="O83" s="1"/>
       <c r="P83" s="1"/>
@@ -5081,18 +5215,28 @@
     <row r="84" ht="12.75" customHeight="1">
       <c r="A84" s="1"/>
       <c r="B84" s="1"/>
-      <c r="C84" s="1"/>
-      <c r="D84" s="1"/>
+      <c r="C84" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="D84" s="9" t="s">
+        <v>231</v>
+      </c>
       <c r="E84" s="1"/>
       <c r="F84" s="1"/>
       <c r="G84" s="1"/>
       <c r="H84" s="1"/>
-      <c r="I84" s="1"/>
+      <c r="I84" s="9" t="s">
+        <v>19</v>
+      </c>
       <c r="J84" s="1"/>
       <c r="K84" s="1"/>
       <c r="L84" s="1"/>
-      <c r="M84" s="1"/>
-      <c r="N84" s="1"/>
+      <c r="M84" s="9" t="s">
+        <v>219</v>
+      </c>
+      <c r="N84" s="9" t="s">
+        <v>28</v>
+      </c>
       <c r="O84" s="1"/>
       <c r="P84" s="1"/>
       <c r="Q84" s="1"/>
@@ -5110,8 +5254,12 @@
     <row r="85" ht="12.75" customHeight="1">
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
-      <c r="C85" s="1"/>
-      <c r="D85" s="1"/>
+      <c r="C85" s="9" t="s">
+        <v>232</v>
+      </c>
+      <c r="D85" s="9" t="s">
+        <v>229</v>
+      </c>
       <c r="E85" s="1"/>
       <c r="F85" s="1"/>
       <c r="G85" s="1"/>
@@ -5120,7 +5268,9 @@
       <c r="J85" s="1"/>
       <c r="K85" s="1"/>
       <c r="L85" s="1"/>
-      <c r="M85" s="1"/>
+      <c r="M85" s="9" t="s">
+        <v>45</v>
+      </c>
       <c r="N85" s="1"/>
       <c r="O85" s="1"/>
       <c r="P85" s="1"/>
@@ -5136,34 +5286,13 @@
       <c r="Z85" s="2"/>
       <c r="AA85" s="2"/>
     </row>
-    <row r="86" ht="12.75" customHeight="1">
-      <c r="A86" s="1"/>
-      <c r="B86" s="1"/>
-      <c r="C86" s="1"/>
-      <c r="D86" s="1"/>
-      <c r="E86" s="1"/>
-      <c r="F86" s="1"/>
-      <c r="G86" s="1"/>
-      <c r="H86" s="1"/>
-      <c r="I86" s="1"/>
-      <c r="J86" s="1"/>
-      <c r="K86" s="1"/>
-      <c r="L86" s="1"/>
-      <c r="M86" s="1"/>
-      <c r="N86" s="1"/>
-      <c r="O86" s="1"/>
-      <c r="P86" s="1"/>
-      <c r="Q86" s="1"/>
-      <c r="R86" s="1"/>
-      <c r="S86" s="1"/>
-      <c r="T86" s="1"/>
-      <c r="U86" s="2"/>
-      <c r="V86" s="2"/>
-      <c r="W86" s="2"/>
-      <c r="X86" s="2"/>
-      <c r="Y86" s="2"/>
-      <c r="Z86" s="2"/>
-      <c r="AA86" s="2"/>
+    <row r="86">
+      <c r="C86" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="87" ht="12.75" customHeight="1">
       <c r="A87" s="1"/>
@@ -10298,7 +10427,7 @@
       <c r="Z263" s="2"/>
       <c r="AA263" s="2"/>
     </row>
-    <row r="264" ht="15.75" customHeight="1">
+    <row r="264" ht="12.75" customHeight="1">
       <c r="A264" s="1"/>
       <c r="B264" s="1"/>
       <c r="C264" s="1"/>
@@ -10705,26 +10834,26 @@
       <c r="AA277" s="2"/>
     </row>
     <row r="278" ht="15.75" customHeight="1">
-      <c r="A278" s="2"/>
-      <c r="B278" s="2"/>
-      <c r="C278" s="2"/>
-      <c r="D278" s="2"/>
-      <c r="E278" s="2"/>
-      <c r="F278" s="2"/>
-      <c r="G278" s="2"/>
-      <c r="H278" s="2"/>
-      <c r="I278" s="2"/>
-      <c r="J278" s="2"/>
-      <c r="K278" s="2"/>
-      <c r="L278" s="2"/>
-      <c r="M278" s="2"/>
-      <c r="N278" s="2"/>
-      <c r="O278" s="2"/>
-      <c r="P278" s="2"/>
-      <c r="Q278" s="2"/>
-      <c r="R278" s="2"/>
-      <c r="S278" s="2"/>
-      <c r="T278" s="2"/>
+      <c r="A278" s="1"/>
+      <c r="B278" s="1"/>
+      <c r="C278" s="1"/>
+      <c r="D278" s="1"/>
+      <c r="E278" s="1"/>
+      <c r="F278" s="1"/>
+      <c r="G278" s="1"/>
+      <c r="H278" s="1"/>
+      <c r="I278" s="1"/>
+      <c r="J278" s="1"/>
+      <c r="K278" s="1"/>
+      <c r="L278" s="1"/>
+      <c r="M278" s="1"/>
+      <c r="N278" s="1"/>
+      <c r="O278" s="1"/>
+      <c r="P278" s="1"/>
+      <c r="Q278" s="1"/>
+      <c r="R278" s="1"/>
+      <c r="S278" s="1"/>
+      <c r="T278" s="1"/>
       <c r="U278" s="2"/>
       <c r="V278" s="2"/>
       <c r="W278" s="2"/>
@@ -31671,8 +31800,37 @@
       <c r="Z1000" s="2"/>
       <c r="AA1000" s="2"/>
     </row>
+    <row r="1001" ht="15.75" customHeight="1">
+      <c r="A1001" s="2"/>
+      <c r="B1001" s="2"/>
+      <c r="C1001" s="2"/>
+      <c r="D1001" s="2"/>
+      <c r="E1001" s="2"/>
+      <c r="F1001" s="2"/>
+      <c r="G1001" s="2"/>
+      <c r="H1001" s="2"/>
+      <c r="I1001" s="2"/>
+      <c r="J1001" s="2"/>
+      <c r="K1001" s="2"/>
+      <c r="L1001" s="2"/>
+      <c r="M1001" s="2"/>
+      <c r="N1001" s="2"/>
+      <c r="O1001" s="2"/>
+      <c r="P1001" s="2"/>
+      <c r="Q1001" s="2"/>
+      <c r="R1001" s="2"/>
+      <c r="S1001" s="2"/>
+      <c r="T1001" s="2"/>
+      <c r="U1001" s="2"/>
+      <c r="V1001" s="2"/>
+      <c r="W1001" s="2"/>
+      <c r="X1001" s="2"/>
+      <c r="Y1001" s="2"/>
+      <c r="Z1001" s="2"/>
+      <c r="AA1001" s="2"/>
+    </row>
   </sheetData>
-  <autoFilter ref="$A$1:$N$79"/>
+  <autoFilter ref="$A$1:$N$86"/>
   <printOptions/>
   <pageMargins bottom="1.05277777777778" footer="0.0" header="0.0" left="0.7875" right="0.7875" top="1.05277777777778"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
add chapter by Vasiliy
</commit_message>
<xml_diff>
--- a/data/contributors.xlsx
+++ b/data/contributors.xlsx
@@ -4204,7 +4204,9 @@
       <c r="A58" s="9">
         <v>57.0</v>
       </c>
-      <c r="B58" s="1"/>
+      <c r="B58" s="3" t="b">
+        <v>1</v>
+      </c>
       <c r="C58" s="9" t="s">
         <v>180</v>
       </c>

</xml_diff>